<commit_message>
Chemistry Coursework - CHANGE PLANNING IMAGE SIZES
</commit_message>
<xml_diff>
--- a/LaTeX/Experiment/Results/Catalysed.xlsx
+++ b/LaTeX/Experiment/Results/Catalysed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="20730" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="720" yWindow="465" windowWidth="20730" windowHeight="11700" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="0.2 Molar" sheetId="1" r:id="rId1"/>
@@ -15,15 +15,12 @@
     <sheet name="1.2 Molar" sheetId="7" r:id="rId6"/>
     <sheet name="ALL" sheetId="8" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="6">
   <si>
     <t>Volume of Hydrogen Produced (ml)</t>
   </si>
@@ -38,6 +35,9 @@
   </si>
   <si>
     <t>Repeat 3</t>
+  </si>
+  <si>
+    <t>Gradient</t>
   </si>
 </sst>
 </file>
@@ -234,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -259,6 +259,8 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -316,7 +318,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -328,6 +329,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="22225"/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
@@ -424,16 +438,18 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116857472"/>
-        <c:axId val="129065728"/>
+        <c:axId val="165282944"/>
+        <c:axId val="165284864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116857472"/>
+        <c:axId val="165282944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -450,14 +466,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129065728"/>
+        <c:crossAx val="165284864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -465,7 +480,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129065728"/>
+        <c:axId val="165284864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -489,14 +504,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116857472"/>
+        <c:crossAx val="165282944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -556,7 +570,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -568,6 +581,20 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="22225"/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
@@ -664,16 +691,18 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="5879680"/>
-        <c:axId val="5885952"/>
+        <c:axId val="165740928"/>
+        <c:axId val="165742848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="5879680"/>
+        <c:axId val="165740928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -690,14 +719,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5885952"/>
+        <c:crossAx val="165742848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -705,7 +733,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5885952"/>
+        <c:axId val="165742848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -729,14 +757,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="5879680"/>
+        <c:crossAx val="165740928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -796,7 +823,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -808,6 +834,20 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="22225"/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
@@ -904,16 +944,18 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="78257536"/>
-        <c:axId val="78390784"/>
+        <c:axId val="168353792"/>
+        <c:axId val="168355712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78257536"/>
+        <c:axId val="168353792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -930,14 +972,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78390784"/>
+        <c:crossAx val="168355712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -945,7 +986,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78390784"/>
+        <c:axId val="168355712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -969,14 +1010,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78257536"/>
+        <c:crossAx val="168353792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1036,7 +1076,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1048,6 +1087,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="22225"/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
@@ -1144,16 +1196,18 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96486912"/>
-        <c:axId val="96488832"/>
+        <c:axId val="168447360"/>
+        <c:axId val="168449536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96486912"/>
+        <c:axId val="168447360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1170,14 +1224,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96488832"/>
+        <c:crossAx val="168449536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1185,10 +1238,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96488832"/>
+        <c:axId val="168449536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1209,14 +1263,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96486912"/>
+        <c:crossAx val="168447360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1276,7 +1329,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1288,6 +1340,20 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="22225"/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
@@ -1384,16 +1450,18 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98066816"/>
-        <c:axId val="98071680"/>
+        <c:axId val="168700928"/>
+        <c:axId val="168776832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98066816"/>
+        <c:axId val="168700928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1410,14 +1478,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98071680"/>
+        <c:crossAx val="168776832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1425,7 +1492,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98071680"/>
+        <c:axId val="168776832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1449,14 +1516,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98066816"/>
+        <c:crossAx val="168700928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1528,6 +1594,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="22225"/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
@@ -1624,16 +1703,18 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98317056"/>
-        <c:axId val="98318976"/>
+        <c:axId val="175442560"/>
+        <c:axId val="175444736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="98317056"/>
+        <c:axId val="175442560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1657,7 +1738,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98318976"/>
+        <c:crossAx val="175444736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1665,10 +1746,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98318976"/>
+        <c:axId val="175444736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1696,7 +1778,252 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98317056"/>
+        <c:crossAx val="175442560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Progress Graph fo</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>r the Catalysed Zinc and Sulfuric Acid Reaction</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>ALL!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ALL!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="175503616"/>
+        <c:axId val="175976832"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="175503616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sulfuric</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Acid Concentration (mol dm</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="30000"/>
+                  <a:t>-3</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="175976832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="175976832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Rate (mol dm</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="30000"/>
+                  <a:t>-3</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>s</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="30000"/>
+                  <a:t>-1</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="175503616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1747,6 +2074,51 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>52552</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>137949</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>512380</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>32845</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9525000" y="1780190"/>
+          <a:ext cx="6568966" cy="2496207"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1782,6 +2154,51 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>55145</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>41413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>298174</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>145382</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9513884" y="2915478"/>
+          <a:ext cx="3307594" cy="2588752"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1821,6 +2238,51 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>69245</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9067800" y="2095500"/>
+          <a:ext cx="3867150" cy="2602895"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1858,6 +2320,51 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>29308</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>527538</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>59722</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9398977" y="1897673"/>
+          <a:ext cx="2294792" cy="2624145"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1893,6 +2400,51 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>53578</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>21981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>241788</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9454020" y="1890346"/>
+          <a:ext cx="2620749" cy="2619375"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1935,141 +2487,84 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="2Molar"/>
-      <sheetName val="2.4Molar"/>
-      <sheetName val="2.8Molar"/>
-      <sheetName val="3.2Molar"/>
-      <sheetName val="3.6Molar"/>
-      <sheetName val="4Molar"/>
-      <sheetName val="All"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="5">
-          <cell r="B5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>30</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>60</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>120</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>150</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>180</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>210</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>240</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>270</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>300</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5">
-        <row r="5">
-          <cell r="M5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="M6">
-            <v>8.6666666666666661</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="M7">
-            <v>20.333333333333332</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="M8">
-            <v>30</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="M9">
-            <v>39</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="M10">
-            <v>49.833333333333336</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="M11">
-            <v>58.833333333333336</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="M12">
-            <v>66.5</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="M13">
-            <v>74.5</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="M14">
-            <v>79</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="M15">
-            <v>85.833333333333329</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.08717</cdr:x>
+      <cdr:y>0.25352</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.3723</cdr:x>
+      <cdr:y>0.86872</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="2" name="Straight Connector 1"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
+          <a:off x="650327" y="1086934"/>
+          <a:ext cx="2127317" cy="2637669"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050"/>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2359,10 +2854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K15"/>
+  <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,6 +3225,15 @@
       </c>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <f>97/100</f>
+        <v>0.97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2738,10 +3242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L15"/>
+  <dimension ref="B1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="H7" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2820,7 +3324,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="9">
-        <f t="shared" ref="I4:J14" si="0">E4-4</f>
+        <f t="shared" ref="J4:J14" si="0">E4-4</f>
         <v>0</v>
       </c>
       <c r="L4">
@@ -3159,6 +3663,15 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <f>100/51.5</f>
+        <v>1.941747572815534</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3167,10 +3680,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L15"/>
+  <dimension ref="B1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3588,6 +4101,15 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <f>100/59</f>
+        <v>1.6949152542372881</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3596,10 +4118,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L15"/>
+  <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4016,6 +4538,15 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <f>100/30.7</f>
+        <v>3.2573289902280131</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4024,10 +4555,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L15"/>
+  <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4445,6 +4976,15 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <f>100/40</f>
+        <v>2.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4453,10 +4993,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L15"/>
+  <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView topLeftCell="H1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4874,6 +5414,12 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <f>100/34.5</f>
+        <v>2.8985507246376812</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4882,10 +5428,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4894,7 +5440,57 @@
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="21">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="21">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="21">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.8</v>
+      </c>
+      <c r="C6" s="21">
+        <v>3.26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="20">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1.2</v>
+      </c>
+      <c r="C8" s="21">
+        <v>2.9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More Chemistry Feedback Improvments
</commit_message>
<xml_diff>
--- a/LaTeX/Experiment/Results/Catalysed.xlsx
+++ b/LaTeX/Experiment/Results/Catalysed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="525" windowWidth="20730" windowHeight="11640" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="720" yWindow="525" windowWidth="20730" windowHeight="11640" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="0.2 Molar" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="9">
   <si>
     <t>Volume of Hydrogen Produced (ml)</t>
   </si>
@@ -43,29 +43,11 @@
     <t>Sulfuric Acid Concentration (Molar)</t>
   </si>
   <si>
+    <t>Average</t>
+  </si>
+  <si>
     <r>
-      <t>Initial Rate of Reaction (mol dm</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> s</t>
+      <t>Initial Rate of Reaction (ml s</t>
     </r>
     <r>
       <rPr>
@@ -94,9 +76,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -293,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -329,8 +310,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,7 +370,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -415,7 +396,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
+              <c:f>'0.2 Molar'!$H$4:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -509,11 +490,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="82446208"/>
-        <c:axId val="82468864"/>
+        <c:axId val="107095936"/>
+        <c:axId val="107106304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82446208"/>
+        <c:axId val="107095936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -537,7 +518,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -554,7 +534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82468864"/>
+        <c:crossAx val="107106304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -562,7 +542,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82468864"/>
+        <c:axId val="107106304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -586,7 +566,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -603,7 +582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82446208"/>
+        <c:crossAx val="107095936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -663,7 +642,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -691,7 +669,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
+              <c:f>'0.2 Molar'!$H$4:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -785,11 +763,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83723776"/>
-        <c:axId val="83725696"/>
+        <c:axId val="108623360"/>
+        <c:axId val="108625280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83723776"/>
+        <c:axId val="108623360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -813,7 +791,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -830,7 +807,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83725696"/>
+        <c:crossAx val="108625280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -838,7 +815,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83725696"/>
+        <c:axId val="108625280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -862,7 +839,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -879,7 +855,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83723776"/>
+        <c:crossAx val="108623360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -939,7 +915,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -967,7 +942,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
+              <c:f>'0.2 Molar'!$H$4:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1061,11 +1036,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84030592"/>
-        <c:axId val="84032512"/>
+        <c:axId val="109716608"/>
+        <c:axId val="109718528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84030592"/>
+        <c:axId val="109716608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,7 +1064,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1106,7 +1080,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84032512"/>
+        <c:crossAx val="109718528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1114,7 +1088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84032512"/>
+        <c:axId val="109718528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1138,7 +1112,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1155,7 +1128,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84030592"/>
+        <c:crossAx val="109716608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1215,7 +1188,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1242,7 +1214,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
+              <c:f>'0.2 Molar'!$H$4:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1336,11 +1308,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83854080"/>
-        <c:axId val="83856000"/>
+        <c:axId val="108446464"/>
+        <c:axId val="108448384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83854080"/>
+        <c:axId val="108446464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1364,7 +1336,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1381,7 +1352,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83856000"/>
+        <c:crossAx val="108448384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1389,7 +1360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83856000"/>
+        <c:axId val="108448384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1414,7 +1385,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1431,7 +1401,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83854080"/>
+        <c:crossAx val="108446464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1491,7 +1461,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1519,7 +1488,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
+              <c:f>'0.2 Molar'!$H$4:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1613,11 +1582,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83904384"/>
-        <c:axId val="83906560"/>
+        <c:axId val="108480000"/>
+        <c:axId val="108481920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83904384"/>
+        <c:axId val="108480000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,7 +1610,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1658,7 +1626,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83906560"/>
+        <c:crossAx val="108481920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1666,7 +1634,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83906560"/>
+        <c:axId val="108481920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1690,7 +1658,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1707,7 +1674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83904384"/>
+        <c:crossAx val="108480000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1767,7 +1734,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1794,7 +1760,7 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'0.2 Molar'!$G$4:$G$14</c:f>
+              <c:f>'0.2 Molar'!$H$4:$H$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1888,11 +1854,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83985920"/>
-        <c:axId val="83987840"/>
+        <c:axId val="108561536"/>
+        <c:axId val="108563456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83985920"/>
+        <c:axId val="108561536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1916,7 +1882,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1933,7 +1898,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83987840"/>
+        <c:crossAx val="108563456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1941,7 +1906,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83987840"/>
+        <c:axId val="108563456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1966,7 +1931,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1983,7 +1947,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83985920"/>
+        <c:crossAx val="108561536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2089,7 +2053,7 @@
             <c:numRef>
               <c:f>ALL!$C$3:$C$8</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0.97</c:v>
@@ -2124,11 +2088,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="84165760"/>
-        <c:axId val="84167680"/>
+        <c:axId val="108588032"/>
+        <c:axId val="109790336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84165760"/>
+        <c:axId val="108588032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2180,7 +2144,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84167680"/>
+        <c:crossAx val="109790336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2188,7 +2152,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84167680"/>
+        <c:axId val="109790336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2234,7 +2198,7 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2248,7 +2212,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84165760"/>
+        <c:crossAx val="108588032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3081,8 +3045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="H2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3100,12 +3064,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -3120,13 +3085,16 @@
       <c r="E3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3143,19 +3111,23 @@
       <c r="E4" s="14">
         <v>2</v>
       </c>
-      <c r="G4" s="8">
+      <c r="F4" s="25">
+        <f>SUM(C4:D4)/2</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" s="9">
-        <f>C4-1</f>
+      <c r="I4" s="9">
+        <f t="shared" ref="I4:I14" si="0">C4-1</f>
         <v>0</v>
       </c>
-      <c r="I4" s="9">
-        <f>D4-1</f>
+      <c r="J4" s="9">
+        <f t="shared" ref="J4:J14" si="1">D4-1</f>
         <v>0</v>
       </c>
       <c r="K4">
-        <f>(H4+I4)/2</f>
+        <f t="shared" ref="K4:K14" si="2">(I4+J4)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3172,19 +3144,23 @@
       <c r="E5" s="15">
         <v>10</v>
       </c>
-      <c r="G5" s="11">
+      <c r="F5" s="25">
+        <f t="shared" ref="F5:F14" si="3">SUM(C5:D5)/2</f>
+        <v>8.25</v>
+      </c>
+      <c r="H5" s="11">
         <v>10</v>
-      </c>
-      <c r="H5" s="9">
-        <f t="shared" ref="H5:I14" si="0">C5-1</f>
-        <v>7.5</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K14" si="1">(H5+I5)/2</f>
+        <f t="shared" si="2"/>
         <v>7.25</v>
       </c>
     </row>
@@ -3201,19 +3177,23 @@
       <c r="E6" s="15">
         <v>15.5</v>
       </c>
-      <c r="G6" s="11">
+      <c r="F6" s="25">
+        <f t="shared" si="3"/>
+        <v>14.5</v>
+      </c>
+      <c r="H6" s="11">
         <v>20</v>
       </c>
-      <c r="H6" s="9">
+      <c r="I6" s="9">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="I6" s="9">
-        <f t="shared" si="0"/>
+      <c r="J6" s="9">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.5</v>
       </c>
     </row>
@@ -3230,19 +3210,23 @@
       <c r="E7" s="15">
         <v>20</v>
       </c>
-      <c r="G7" s="11">
+      <c r="F7" s="25">
+        <f t="shared" si="3"/>
+        <v>17.5</v>
+      </c>
+      <c r="H7" s="11">
         <v>30</v>
       </c>
-      <c r="H7" s="9">
+      <c r="I7" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I7" s="9">
-        <f t="shared" si="0"/>
+      <c r="J7" s="9">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16.5</v>
       </c>
     </row>
@@ -3259,19 +3243,23 @@
       <c r="E8" s="15">
         <v>25.5</v>
       </c>
-      <c r="G8" s="11">
+      <c r="F8" s="25">
+        <f t="shared" si="3"/>
+        <v>20.25</v>
+      </c>
+      <c r="H8" s="11">
         <v>40</v>
       </c>
-      <c r="H8" s="9">
+      <c r="I8" s="9">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="I8" s="9">
-        <f t="shared" si="0"/>
+      <c r="J8" s="9">
+        <f t="shared" si="1"/>
         <v>19.5</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19.25</v>
       </c>
     </row>
@@ -3288,19 +3276,23 @@
       <c r="E9" s="15">
         <v>30</v>
       </c>
-      <c r="G9" s="11">
+      <c r="F9" s="25">
+        <f t="shared" si="3"/>
+        <v>22.5</v>
+      </c>
+      <c r="H9" s="11">
         <v>50</v>
-      </c>
-      <c r="H9" s="9">
-        <f t="shared" si="0"/>
-        <v>21.5</v>
       </c>
       <c r="I9" s="9">
         <f t="shared" si="0"/>
         <v>21.5</v>
       </c>
+      <c r="J9" s="9">
+        <f t="shared" si="1"/>
+        <v>21.5</v>
+      </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21.5</v>
       </c>
     </row>
@@ -3317,19 +3309,23 @@
       <c r="E10" s="15">
         <v>32.5</v>
       </c>
-      <c r="G10" s="11">
+      <c r="F10" s="25">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="H10" s="11">
         <v>60</v>
-      </c>
-      <c r="H10" s="9">
-        <f t="shared" si="0"/>
-        <v>23</v>
       </c>
       <c r="I10" s="9">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
+      <c r="J10" s="9">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
       <c r="K10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
     </row>
@@ -3346,19 +3342,23 @@
       <c r="E11" s="15">
         <v>36</v>
       </c>
-      <c r="G11" s="11">
+      <c r="F11" s="25">
+        <f t="shared" si="3"/>
+        <v>25.25</v>
+      </c>
+      <c r="H11" s="11">
         <v>70</v>
       </c>
-      <c r="H11" s="9">
+      <c r="I11" s="9">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="I11" s="9">
-        <f t="shared" si="0"/>
+      <c r="J11" s="9">
+        <f t="shared" si="1"/>
         <v>24.5</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24.25</v>
       </c>
     </row>
@@ -3375,19 +3375,23 @@
       <c r="E12" s="15">
         <v>38</v>
       </c>
-      <c r="G12" s="11">
+      <c r="F12" s="25">
+        <f t="shared" si="3"/>
+        <v>26.25</v>
+      </c>
+      <c r="H12" s="11">
         <v>80</v>
       </c>
-      <c r="H12" s="9">
+      <c r="I12" s="9">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="I12" s="9">
-        <f t="shared" si="0"/>
+      <c r="J12" s="9">
+        <f t="shared" si="1"/>
         <v>25.5</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.25</v>
       </c>
     </row>
@@ -3404,19 +3408,23 @@
       <c r="E13" s="15">
         <v>40</v>
       </c>
-      <c r="G13" s="11">
+      <c r="F13" s="25">
+        <f t="shared" si="3"/>
+        <v>27.5</v>
+      </c>
+      <c r="H13" s="11">
         <v>90</v>
-      </c>
-      <c r="H13" s="9">
-        <f t="shared" si="0"/>
-        <v>26.5</v>
       </c>
       <c r="I13" s="9">
         <f t="shared" si="0"/>
         <v>26.5</v>
       </c>
+      <c r="J13" s="9">
+        <f t="shared" si="1"/>
+        <v>26.5</v>
+      </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26.5</v>
       </c>
     </row>
@@ -3433,19 +3441,23 @@
       <c r="E14" s="15">
         <v>42.5</v>
       </c>
-      <c r="G14" s="11">
+      <c r="F14" s="25">
+        <f t="shared" si="3"/>
+        <v>28.75</v>
+      </c>
+      <c r="H14" s="11">
         <v>100</v>
       </c>
-      <c r="H14" s="9">
+      <c r="I14" s="9">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="I14" s="9">
-        <f t="shared" si="0"/>
+      <c r="J14" s="9">
+        <f t="shared" si="1"/>
         <v>27.5</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27.75</v>
       </c>
     </row>
@@ -3469,8 +3481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="I8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3491,12 +3503,13 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="3"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -3511,16 +3524,19 @@
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3537,23 +3553,27 @@
       <c r="E4" s="10">
         <v>4</v>
       </c>
-      <c r="G4" s="8">
+      <c r="F4" s="25">
+        <f>SUM(C4:E4)/3</f>
+        <v>3.8333333333333335</v>
+      </c>
+      <c r="H4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" s="9">
-        <f>C4-4</f>
+      <c r="I4" s="9">
+        <f t="shared" ref="I4:I14" si="0">C4-4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="9">
-        <f>D4-3.5</f>
+      <c r="J4" s="9">
+        <f t="shared" ref="J4:J14" si="1">D4-3.5</f>
         <v>0</v>
       </c>
-      <c r="J4" s="9">
-        <f t="shared" ref="J4:J14" si="0">E4-4</f>
+      <c r="K4" s="9">
+        <f t="shared" ref="K4:K14" si="2">E4-4</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>(H4+I4+J4)/3</f>
+        <f t="shared" ref="L4:L14" si="3">(I4+J4+K4)/3</f>
         <v>0</v>
       </c>
     </row>
@@ -3570,23 +3590,27 @@
       <c r="E5" s="13">
         <v>20</v>
       </c>
-      <c r="G5" s="11">
+      <c r="F5" s="25">
+        <f t="shared" ref="F5:F14" si="4">SUM(C5:E5)/3</f>
+        <v>19.833333333333332</v>
+      </c>
+      <c r="H5" s="11">
         <v>10</v>
       </c>
-      <c r="H5" s="9">
-        <f t="shared" ref="H5:H14" si="1">C5-4</f>
+      <c r="I5" s="9">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="I5" s="9">
-        <f t="shared" ref="I5:I14" si="2">D5-3.5</f>
+      <c r="J5" s="9">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="J5" s="9">
-        <f t="shared" si="0"/>
+      <c r="K5" s="9">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L14" si="3">(H5+I5+J5)/3</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
     </row>
@@ -3603,19 +3627,23 @@
       <c r="E6" s="13">
         <v>27.5</v>
       </c>
-      <c r="G6" s="11">
+      <c r="F6" s="25">
+        <f t="shared" si="4"/>
+        <v>27.5</v>
+      </c>
+      <c r="H6" s="11">
         <v>20</v>
       </c>
-      <c r="H6" s="9">
+      <c r="I6" s="9">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="J6" s="9">
         <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="I6" s="9">
+        <v>24.5</v>
+      </c>
+      <c r="K6" s="9">
         <f t="shared" si="2"/>
-        <v>24.5</v>
-      </c>
-      <c r="J6" s="9">
-        <f t="shared" si="0"/>
         <v>23.5</v>
       </c>
       <c r="L6">
@@ -3636,19 +3664,23 @@
       <c r="E7" s="13">
         <v>33.5</v>
       </c>
-      <c r="G7" s="11">
+      <c r="F7" s="25">
+        <f t="shared" si="4"/>
+        <v>33.5</v>
+      </c>
+      <c r="H7" s="11">
         <v>30</v>
       </c>
-      <c r="H7" s="9">
+      <c r="I7" s="9">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="J7" s="9">
         <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="I7" s="9">
+        <v>30.5</v>
+      </c>
+      <c r="K7" s="9">
         <f t="shared" si="2"/>
-        <v>30.5</v>
-      </c>
-      <c r="J7" s="9">
-        <f t="shared" si="0"/>
         <v>29.5</v>
       </c>
       <c r="L7">
@@ -3669,19 +3701,23 @@
       <c r="E8" s="13">
         <v>39.5</v>
       </c>
-      <c r="G8" s="11">
+      <c r="F8" s="25">
+        <f t="shared" si="4"/>
+        <v>39.333333333333336</v>
+      </c>
+      <c r="H8" s="11">
         <v>40</v>
       </c>
-      <c r="H8" s="9">
+      <c r="I8" s="9">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="J8" s="9">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="I8" s="9">
+        <v>36</v>
+      </c>
+      <c r="K8" s="9">
         <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="J8" s="9">
-        <f t="shared" si="0"/>
         <v>35.5</v>
       </c>
       <c r="L8">
@@ -3702,19 +3738,23 @@
       <c r="E9" s="13">
         <v>45</v>
       </c>
-      <c r="G9" s="11">
+      <c r="F9" s="25">
+        <f t="shared" si="4"/>
+        <v>44.666666666666664</v>
+      </c>
+      <c r="H9" s="11">
         <v>50</v>
       </c>
-      <c r="H9" s="9">
+      <c r="I9" s="9">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="J9" s="9">
         <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="I9" s="9">
+        <v>41.5</v>
+      </c>
+      <c r="K9" s="9">
         <f t="shared" si="2"/>
-        <v>41.5</v>
-      </c>
-      <c r="J9" s="9">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="L9">
@@ -3735,19 +3775,23 @@
       <c r="E10" s="13">
         <v>50</v>
       </c>
-      <c r="G10" s="11">
+      <c r="F10" s="25">
+        <f t="shared" si="4"/>
+        <v>49.833333333333336</v>
+      </c>
+      <c r="H10" s="11">
         <v>60</v>
       </c>
-      <c r="H10" s="9">
+      <c r="I10" s="9">
+        <f t="shared" si="0"/>
+        <v>45.5</v>
+      </c>
+      <c r="J10" s="9">
         <f t="shared" si="1"/>
-        <v>45.5</v>
-      </c>
-      <c r="I10" s="9">
+        <v>46.5</v>
+      </c>
+      <c r="K10" s="9">
         <f t="shared" si="2"/>
-        <v>46.5</v>
-      </c>
-      <c r="J10" s="9">
-        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="L10">
@@ -3768,19 +3812,23 @@
       <c r="E11" s="13">
         <v>53.5</v>
       </c>
-      <c r="G11" s="11">
+      <c r="F11" s="25">
+        <f t="shared" si="4"/>
+        <v>53.666666666666664</v>
+      </c>
+      <c r="H11" s="11">
         <v>70</v>
       </c>
-      <c r="H11" s="9">
+      <c r="I11" s="9">
+        <f t="shared" si="0"/>
+        <v>48.5</v>
+      </c>
+      <c r="J11" s="9">
         <f t="shared" si="1"/>
-        <v>48.5</v>
-      </c>
-      <c r="I11" s="9">
+        <v>51.5</v>
+      </c>
+      <c r="K11" s="9">
         <f t="shared" si="2"/>
-        <v>51.5</v>
-      </c>
-      <c r="J11" s="9">
-        <f t="shared" si="0"/>
         <v>49.5</v>
       </c>
       <c r="L11">
@@ -3801,19 +3849,23 @@
       <c r="E12" s="13">
         <v>57</v>
       </c>
-      <c r="G12" s="11">
+      <c r="F12" s="25">
+        <f t="shared" si="4"/>
+        <v>57.5</v>
+      </c>
+      <c r="H12" s="11">
         <v>80</v>
       </c>
-      <c r="H12" s="9">
+      <c r="I12" s="9">
+        <f t="shared" si="0"/>
+        <v>52.5</v>
+      </c>
+      <c r="J12" s="9">
         <f t="shared" si="1"/>
-        <v>52.5</v>
-      </c>
-      <c r="I12" s="9">
+        <v>55.5</v>
+      </c>
+      <c r="K12" s="9">
         <f t="shared" si="2"/>
-        <v>55.5</v>
-      </c>
-      <c r="J12" s="9">
-        <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="L12">
@@ -3834,19 +3886,23 @@
       <c r="E13" s="13">
         <v>61</v>
       </c>
-      <c r="G13" s="11">
+      <c r="F13" s="25">
+        <f t="shared" si="4"/>
+        <v>61.166666666666664</v>
+      </c>
+      <c r="H13" s="11">
         <v>90</v>
       </c>
-      <c r="H13" s="9">
+      <c r="I13" s="9">
+        <f t="shared" si="0"/>
+        <v>56.5</v>
+      </c>
+      <c r="J13" s="9">
         <f t="shared" si="1"/>
-        <v>56.5</v>
-      </c>
-      <c r="I13" s="9">
+        <v>58.5</v>
+      </c>
+      <c r="K13" s="9">
         <f t="shared" si="2"/>
-        <v>58.5</v>
-      </c>
-      <c r="J13" s="9">
-        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="L13">
@@ -3867,19 +3923,23 @@
       <c r="E14" s="13">
         <v>64.5</v>
       </c>
-      <c r="G14" s="11">
+      <c r="F14" s="25">
+        <f t="shared" si="4"/>
+        <v>64.5</v>
+      </c>
+      <c r="H14" s="11">
         <v>100</v>
       </c>
-      <c r="H14" s="9">
+      <c r="I14" s="9">
+        <f t="shared" si="0"/>
+        <v>59.5</v>
+      </c>
+      <c r="J14" s="9">
         <f t="shared" si="1"/>
-        <v>59.5</v>
-      </c>
-      <c r="I14" s="9">
+        <v>62</v>
+      </c>
+      <c r="K14" s="9">
         <f t="shared" si="2"/>
-        <v>62</v>
-      </c>
-      <c r="J14" s="9">
-        <f t="shared" si="0"/>
         <v>60.5</v>
       </c>
       <c r="L14">
@@ -3907,8 +3967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="H4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3929,12 +3989,13 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="3"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -3949,16 +4010,19 @@
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3975,23 +4039,27 @@
       <c r="E4" s="10">
         <v>5</v>
       </c>
-      <c r="G4" s="8">
+      <c r="F4" s="25">
+        <f>SUM(D4:E4)/2</f>
+        <v>6</v>
+      </c>
+      <c r="H4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" s="17">
-        <f>C4-3.5</f>
+      <c r="I4" s="17">
+        <f t="shared" ref="I4:I14" si="0">C4-3.5</f>
         <v>0</v>
       </c>
-      <c r="I4" s="10">
-        <f>D4-7</f>
+      <c r="J4" s="10">
+        <f t="shared" ref="J4:J14" si="1">D4-7</f>
         <v>0</v>
       </c>
-      <c r="J4" s="10">
-        <f>E4-5</f>
+      <c r="K4" s="10">
+        <f t="shared" ref="K4:K14" si="2">E4-5</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>(I4+J4)/2</f>
+        <f t="shared" ref="L4:L14" si="3">(J4+K4)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -4008,23 +4076,27 @@
       <c r="E5" s="13">
         <v>18</v>
       </c>
-      <c r="G5" s="11">
+      <c r="F5" s="25">
+        <f t="shared" ref="F5:F14" si="4">SUM(D5:E5)/2</f>
+        <v>19</v>
+      </c>
+      <c r="H5" s="11">
         <v>10</v>
       </c>
-      <c r="H5" s="17">
-        <f t="shared" ref="H5:H14" si="0">C5-3.5</f>
+      <c r="I5" s="17">
+        <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
-      <c r="I5" s="10">
-        <f t="shared" ref="I5:I14" si="1">D5-7</f>
+      <c r="J5" s="10">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J5" s="10">
-        <f t="shared" ref="J5:J14" si="2">E5-5</f>
+      <c r="K5" s="10">
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L14" si="3">(I5+J5)/2</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
     </row>
@@ -4041,18 +4113,22 @@
       <c r="E6" s="13">
         <v>25.5</v>
       </c>
-      <c r="G6" s="11">
+      <c r="F6" s="25">
+        <f t="shared" si="4"/>
+        <v>26.25</v>
+      </c>
+      <c r="H6" s="11">
         <v>20</v>
       </c>
-      <c r="H6" s="17">
+      <c r="I6" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="I6" s="10">
+      <c r="J6" s="10">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="J6" s="10">
+      <c r="K6" s="10">
         <f t="shared" si="2"/>
         <v>20.5</v>
       </c>
@@ -4074,18 +4150,22 @@
       <c r="E7" s="13">
         <v>30.5</v>
       </c>
-      <c r="G7" s="11">
+      <c r="F7" s="25">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="H7" s="11">
         <v>30</v>
       </c>
-      <c r="H7" s="17">
+      <c r="I7" s="17">
         <f t="shared" si="0"/>
         <v>22.5</v>
       </c>
-      <c r="I7" s="10">
+      <c r="J7" s="10">
         <f t="shared" si="1"/>
         <v>26.5</v>
       </c>
-      <c r="J7" s="10">
+      <c r="K7" s="10">
         <f t="shared" si="2"/>
         <v>25.5</v>
       </c>
@@ -4107,18 +4187,22 @@
       <c r="E8" s="13">
         <v>33.5</v>
       </c>
-      <c r="G8" s="11">
+      <c r="F8" s="25">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="H8" s="11">
         <v>40</v>
       </c>
-      <c r="H8" s="17">
+      <c r="I8" s="17">
         <f t="shared" si="0"/>
         <v>31.5</v>
       </c>
-      <c r="I8" s="10">
+      <c r="J8" s="10">
         <f t="shared" si="1"/>
         <v>31.5</v>
       </c>
-      <c r="J8" s="10">
+      <c r="K8" s="10">
         <f t="shared" si="2"/>
         <v>28.5</v>
       </c>
@@ -4140,18 +4224,22 @@
       <c r="E9" s="13">
         <v>41.5</v>
       </c>
-      <c r="G9" s="11">
+      <c r="F9" s="25">
+        <f t="shared" si="4"/>
+        <v>41.75</v>
+      </c>
+      <c r="H9" s="11">
         <v>50</v>
       </c>
-      <c r="H9" s="17">
+      <c r="I9" s="17">
         <f t="shared" si="0"/>
         <v>36.5</v>
       </c>
-      <c r="I9" s="10">
+      <c r="J9" s="10">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="J9" s="10">
+      <c r="K9" s="10">
         <f t="shared" si="2"/>
         <v>36.5</v>
       </c>
@@ -4173,18 +4261,22 @@
       <c r="E10" s="13">
         <v>46</v>
       </c>
-      <c r="G10" s="11">
+      <c r="F10" s="25">
+        <f t="shared" si="4"/>
+        <v>45.75</v>
+      </c>
+      <c r="H10" s="11">
         <v>60</v>
       </c>
-      <c r="H10" s="17">
+      <c r="I10" s="17">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="I10" s="10">
+      <c r="J10" s="10">
         <f t="shared" si="1"/>
         <v>38.5</v>
       </c>
-      <c r="J10" s="10">
+      <c r="K10" s="10">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
@@ -4206,18 +4298,22 @@
       <c r="E11" s="13">
         <v>48.5</v>
       </c>
-      <c r="G11" s="11">
+      <c r="F11" s="25">
+        <f t="shared" si="4"/>
+        <v>48.25</v>
+      </c>
+      <c r="H11" s="11">
         <v>70</v>
       </c>
-      <c r="H11" s="17">
+      <c r="I11" s="17">
         <f t="shared" si="0"/>
         <v>43.5</v>
       </c>
-      <c r="I11" s="10">
+      <c r="J11" s="10">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="J11" s="10">
+      <c r="K11" s="10">
         <f t="shared" si="2"/>
         <v>43.5</v>
       </c>
@@ -4239,18 +4335,22 @@
       <c r="E12" s="13">
         <v>51</v>
       </c>
-      <c r="G12" s="11">
+      <c r="F12" s="25">
+        <f t="shared" si="4"/>
+        <v>51.5</v>
+      </c>
+      <c r="H12" s="11">
         <v>80</v>
       </c>
-      <c r="H12" s="17">
+      <c r="I12" s="17">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="I12" s="10">
+      <c r="J12" s="10">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="J12" s="10">
+      <c r="K12" s="10">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
@@ -4272,18 +4372,22 @@
       <c r="E13" s="13">
         <v>53</v>
       </c>
-      <c r="G13" s="11">
+      <c r="F13" s="25">
+        <f t="shared" si="4"/>
+        <v>53.75</v>
+      </c>
+      <c r="H13" s="11">
         <v>90</v>
       </c>
-      <c r="H13" s="17">
+      <c r="I13" s="17">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="I13" s="10">
+      <c r="J13" s="10">
         <f t="shared" si="1"/>
         <v>47.5</v>
       </c>
-      <c r="J13" s="10">
+      <c r="K13" s="10">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
@@ -4305,18 +4409,22 @@
       <c r="E14" s="13">
         <v>56</v>
       </c>
-      <c r="G14" s="11">
+      <c r="F14" s="25">
+        <f t="shared" si="4"/>
+        <v>57.5</v>
+      </c>
+      <c r="H14" s="11">
         <v>100</v>
       </c>
-      <c r="H14" s="17">
+      <c r="I14" s="17">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="I14" s="10">
+      <c r="J14" s="10">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="J14" s="10">
+      <c r="K14" s="10">
         <f t="shared" si="2"/>
         <v>51</v>
       </c>
@@ -4345,8 +4453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="H3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4365,13 +4473,14 @@
         <v>0</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -4386,16 +4495,19 @@
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4412,23 +4524,27 @@
       <c r="E4" s="10">
         <v>6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="F4" s="25">
+        <f>SUM(C4:E4)/3</f>
+        <v>6</v>
+      </c>
+      <c r="H4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" s="9">
-        <f>C4-6</f>
+      <c r="I4" s="9">
+        <f t="shared" ref="I4:I14" si="0">C4-6</f>
         <v>0</v>
       </c>
-      <c r="I4" s="9">
-        <f t="shared" ref="I4:J14" si="0">D4-6</f>
+      <c r="J4" s="9">
+        <f t="shared" ref="J4:J14" si="1">D4-6</f>
         <v>0</v>
       </c>
-      <c r="J4" s="9">
-        <f t="shared" si="0"/>
+      <c r="K4" s="9">
+        <f t="shared" ref="K4:K14" si="2">E4-6</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>(H4+I4+J4) /3</f>
+        <f t="shared" ref="L4:L14" si="3">(I4+J4+K4) /3</f>
         <v>0</v>
       </c>
     </row>
@@ -4445,23 +4561,27 @@
       <c r="E5" s="13">
         <v>28</v>
       </c>
-      <c r="G5" s="11">
+      <c r="F5" s="25">
+        <f t="shared" ref="F5:F14" si="4">SUM(C5:E5)/3</f>
+        <v>28.5</v>
+      </c>
+      <c r="H5" s="11">
         <v>10</v>
-      </c>
-      <c r="H5" s="9">
-        <f t="shared" ref="H5:H14" si="1">C5-6</f>
-        <v>24</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="1"/>
         <v>21.5</v>
       </c>
-      <c r="J5" s="9">
-        <f t="shared" si="0"/>
+      <c r="K5" s="9">
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L14" si="2">(H5+I5+J5) /3</f>
+        <f t="shared" si="3"/>
         <v>22.5</v>
       </c>
     </row>
@@ -4478,23 +4598,27 @@
       <c r="E6" s="13">
         <v>41</v>
       </c>
-      <c r="G6" s="11">
+      <c r="F6" s="25">
+        <f t="shared" si="4"/>
+        <v>41.833333333333336</v>
+      </c>
+      <c r="H6" s="11">
         <v>20</v>
-      </c>
-      <c r="H6" s="9">
-        <f t="shared" si="1"/>
-        <v>39</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="1"/>
         <v>33.5</v>
       </c>
-      <c r="J6" s="9">
-        <f t="shared" si="0"/>
+      <c r="K6" s="9">
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="L6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35.833333333333336</v>
       </c>
     </row>
@@ -4511,23 +4635,27 @@
       <c r="E7" s="13">
         <v>48.5</v>
       </c>
-      <c r="G7" s="11">
+      <c r="F7" s="25">
+        <f t="shared" si="4"/>
+        <v>49.5</v>
+      </c>
+      <c r="H7" s="11">
         <v>30</v>
-      </c>
-      <c r="H7" s="9">
-        <f t="shared" si="1"/>
-        <v>48</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="J7" s="9">
-        <f t="shared" si="0"/>
+      <c r="K7" s="9">
+        <f t="shared" si="2"/>
         <v>42.5</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43.5</v>
       </c>
     </row>
@@ -4544,23 +4672,27 @@
       <c r="E8" s="13">
         <v>55</v>
       </c>
-      <c r="G8" s="11">
+      <c r="F8" s="25">
+        <f t="shared" si="4"/>
+        <v>55.833333333333336</v>
+      </c>
+      <c r="H8" s="11">
         <v>40</v>
-      </c>
-      <c r="H8" s="9">
-        <f t="shared" si="1"/>
-        <v>54.5</v>
       </c>
       <c r="I8" s="9">
         <f t="shared" si="0"/>
+        <v>54.5</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="J8" s="9">
-        <f t="shared" si="0"/>
+      <c r="K8" s="9">
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="L8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49.833333333333336</v>
       </c>
     </row>
@@ -4577,23 +4709,27 @@
       <c r="E9" s="13">
         <v>60</v>
       </c>
-      <c r="G9" s="11">
+      <c r="F9" s="25">
+        <f t="shared" si="4"/>
+        <v>61.166666666666664</v>
+      </c>
+      <c r="H9" s="11">
         <v>50</v>
-      </c>
-      <c r="H9" s="9">
-        <f t="shared" si="1"/>
-        <v>60</v>
       </c>
       <c r="I9" s="9">
         <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="1"/>
         <v>51.5</v>
       </c>
-      <c r="J9" s="9">
-        <f t="shared" si="0"/>
+      <c r="K9" s="9">
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="L9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55.166666666666664</v>
       </c>
     </row>
@@ -4610,23 +4746,27 @@
       <c r="E10" s="13">
         <v>65.5</v>
       </c>
-      <c r="G10" s="11">
+      <c r="F10" s="25">
+        <f t="shared" si="4"/>
+        <v>65.833333333333329</v>
+      </c>
+      <c r="H10" s="11">
         <v>60</v>
-      </c>
-      <c r="H10" s="9">
-        <f t="shared" si="1"/>
-        <v>64</v>
       </c>
       <c r="I10" s="9">
         <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="J10" s="9">
-        <f t="shared" si="0"/>
+      <c r="K10" s="9">
+        <f t="shared" si="2"/>
         <v>59.5</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>59.833333333333336</v>
       </c>
     </row>
@@ -4643,23 +4783,27 @@
       <c r="E11" s="13">
         <v>70.5</v>
       </c>
-      <c r="G11" s="11">
+      <c r="F11" s="25">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="H11" s="11">
         <v>70</v>
-      </c>
-      <c r="H11" s="9">
-        <f t="shared" si="1"/>
-        <v>69</v>
       </c>
       <c r="I11" s="9">
         <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" si="1"/>
         <v>61.5</v>
       </c>
-      <c r="J11" s="9">
-        <f t="shared" si="0"/>
+      <c r="K11" s="9">
+        <f t="shared" si="2"/>
         <v>64.5</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
     </row>
@@ -4676,23 +4820,27 @@
       <c r="E12" s="13">
         <v>76</v>
       </c>
-      <c r="G12" s="11">
-        <v>80</v>
-      </c>
-      <c r="H12" s="9">
-        <f t="shared" si="1"/>
+      <c r="F12" s="25">
+        <f t="shared" si="4"/>
+        <v>78.333333333333329</v>
+      </c>
+      <c r="H12" s="11">
         <v>80</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="J12" s="9">
-        <f t="shared" si="0"/>
+      <c r="K12" s="9">
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>72.333333333333329</v>
       </c>
     </row>
@@ -4709,23 +4857,27 @@
       <c r="E13" s="13">
         <v>80</v>
       </c>
-      <c r="G13" s="11">
+      <c r="F13" s="25">
+        <f t="shared" si="4"/>
+        <v>80.5</v>
+      </c>
+      <c r="H13" s="11">
         <v>90</v>
-      </c>
-      <c r="H13" s="9">
-        <f t="shared" si="1"/>
-        <v>78.5</v>
       </c>
       <c r="I13" s="9">
         <f t="shared" si="0"/>
+        <v>78.5</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="J13" s="9">
-        <f t="shared" si="0"/>
+      <c r="K13" s="9">
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>74.5</v>
       </c>
     </row>
@@ -4742,23 +4894,27 @@
       <c r="E14" s="13">
         <v>85</v>
       </c>
-      <c r="G14" s="11">
+      <c r="F14" s="25">
+        <f t="shared" si="4"/>
+        <v>84.333333333333329</v>
+      </c>
+      <c r="H14" s="11">
         <v>100</v>
-      </c>
-      <c r="H14" s="9">
-        <f t="shared" si="1"/>
-        <v>82</v>
       </c>
       <c r="I14" s="9">
         <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="J14" s="9">
+        <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="J14" s="9">
-        <f t="shared" si="0"/>
+      <c r="K14" s="9">
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>78.333333333333329</v>
       </c>
     </row>
@@ -4782,8 +4938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4803,13 +4959,14 @@
         <v>0</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -4824,16 +4981,19 @@
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4850,23 +5010,27 @@
       <c r="E4" s="10">
         <v>8</v>
       </c>
-      <c r="G4" s="8">
+      <c r="F4" s="25">
+        <f>SUM(C4:E4)/3</f>
+        <v>8</v>
+      </c>
+      <c r="H4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" s="9">
-        <f>C4-8</f>
+      <c r="I4" s="9">
+        <f t="shared" ref="I4:I14" si="0">C4-8</f>
         <v>0</v>
       </c>
-      <c r="I4" s="9">
-        <f t="shared" ref="I4:J14" si="0">D4-8</f>
+      <c r="J4" s="9">
+        <f t="shared" ref="J4:J14" si="1">D4-8</f>
         <v>0</v>
       </c>
-      <c r="J4" s="9">
-        <f t="shared" si="0"/>
+      <c r="K4" s="9">
+        <f t="shared" ref="K4:K14" si="2">E4-8</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>(H4+I4+J4)/3</f>
+        <f t="shared" ref="L4:L14" si="3">(I4+J4+K4)/3</f>
         <v>0</v>
       </c>
     </row>
@@ -4883,23 +5047,27 @@
       <c r="E5" s="13">
         <v>29.5</v>
       </c>
-      <c r="G5" s="11">
+      <c r="F5" s="25">
+        <f t="shared" ref="F5:F14" si="4">SUM(C5:E5)/3</f>
+        <v>29.5</v>
+      </c>
+      <c r="H5" s="11">
         <v>10</v>
-      </c>
-      <c r="H5" s="9">
-        <f t="shared" ref="H5:H14" si="1">C5-8</f>
-        <v>21</v>
       </c>
       <c r="I5" s="9">
         <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="J5" s="9">
-        <f t="shared" si="0"/>
+      <c r="K5" s="9">
+        <f t="shared" si="2"/>
         <v>21.5</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L14" si="2">(H5+I5+J5)/3</f>
+        <f t="shared" si="3"/>
         <v>21.5</v>
       </c>
     </row>
@@ -4916,23 +5084,27 @@
       <c r="E6" s="13">
         <v>40</v>
       </c>
-      <c r="G6" s="11">
+      <c r="F6" s="25">
+        <f t="shared" si="4"/>
+        <v>40.333333333333336</v>
+      </c>
+      <c r="H6" s="11">
         <v>20</v>
-      </c>
-      <c r="H6" s="9">
-        <f t="shared" si="1"/>
-        <v>32</v>
       </c>
       <c r="I6" s="9">
         <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="J6" s="9">
-        <f t="shared" si="0"/>
+      <c r="K6" s="9">
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="L6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32.333333333333336</v>
       </c>
     </row>
@@ -4949,23 +5121,27 @@
       <c r="E7" s="13">
         <v>51</v>
       </c>
-      <c r="G7" s="11">
+      <c r="F7" s="25">
+        <f t="shared" si="4"/>
+        <v>50.833333333333336</v>
+      </c>
+      <c r="H7" s="11">
         <v>30</v>
-      </c>
-      <c r="H7" s="9">
-        <f t="shared" si="1"/>
-        <v>43</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="1"/>
         <v>42.5</v>
       </c>
-      <c r="J7" s="9">
-        <f t="shared" si="0"/>
+      <c r="K7" s="9">
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42.833333333333336</v>
       </c>
     </row>
@@ -4982,23 +5158,27 @@
       <c r="E8" s="13">
         <v>60</v>
       </c>
-      <c r="G8" s="11">
+      <c r="F8" s="25">
+        <f t="shared" si="4"/>
+        <v>60.333333333333336</v>
+      </c>
+      <c r="H8" s="11">
         <v>40</v>
-      </c>
-      <c r="H8" s="9">
-        <f t="shared" si="1"/>
-        <v>52</v>
       </c>
       <c r="I8" s="9">
         <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="J8" s="9">
-        <f t="shared" si="0"/>
+      <c r="K8" s="9">
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="L8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>52.333333333333336</v>
       </c>
     </row>
@@ -5015,23 +5195,27 @@
       <c r="E9" s="13">
         <v>66</v>
       </c>
-      <c r="G9" s="11">
+      <c r="F9" s="25">
+        <f t="shared" si="4"/>
+        <v>65.833333333333329</v>
+      </c>
+      <c r="H9" s="11">
         <v>50</v>
-      </c>
-      <c r="H9" s="9">
-        <f t="shared" si="1"/>
-        <v>57.5</v>
       </c>
       <c r="I9" s="9">
         <f t="shared" si="0"/>
+        <v>57.5</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
-      <c r="J9" s="9">
-        <f t="shared" si="0"/>
+      <c r="K9" s="9">
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="L9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57.833333333333336</v>
       </c>
     </row>
@@ -5048,23 +5232,27 @@
       <c r="E10" s="13">
         <v>70.5</v>
       </c>
-      <c r="G10" s="11">
+      <c r="F10" s="25">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="H10" s="11">
         <v>60</v>
-      </c>
-      <c r="H10" s="9">
-        <f t="shared" si="1"/>
-        <v>62.5</v>
       </c>
       <c r="I10" s="9">
         <f t="shared" si="0"/>
+        <v>62.5</v>
+      </c>
+      <c r="J10" s="9">
+        <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="J10" s="9">
-        <f t="shared" si="0"/>
+      <c r="K10" s="9">
+        <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>63</v>
       </c>
     </row>
@@ -5081,23 +5269,27 @@
       <c r="E11" s="13">
         <v>77.5</v>
       </c>
-      <c r="G11" s="11">
+      <c r="F11" s="25">
+        <f t="shared" si="4"/>
+        <v>78.166666666666671</v>
+      </c>
+      <c r="H11" s="11">
         <v>70</v>
-      </c>
-      <c r="H11" s="9">
-        <f t="shared" si="1"/>
-        <v>69</v>
       </c>
       <c r="I11" s="9">
         <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="J11" s="9">
-        <f t="shared" si="0"/>
+      <c r="K11" s="9">
+        <f t="shared" si="2"/>
         <v>69.5</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70.166666666666671</v>
       </c>
     </row>
@@ -5114,23 +5306,27 @@
       <c r="E12" s="13">
         <v>82.5</v>
       </c>
-      <c r="G12" s="11">
+      <c r="F12" s="25">
+        <f t="shared" si="4"/>
+        <v>82.666666666666671</v>
+      </c>
+      <c r="H12" s="11">
         <v>80</v>
-      </c>
-      <c r="H12" s="9">
-        <f t="shared" si="1"/>
-        <v>72.5</v>
       </c>
       <c r="I12" s="9">
         <f t="shared" si="0"/>
+        <v>72.5</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="J12" s="9">
-        <f t="shared" si="0"/>
+      <c r="K12" s="9">
+        <f t="shared" si="2"/>
         <v>74.5</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>74.666666666666671</v>
       </c>
     </row>
@@ -5147,23 +5343,27 @@
       <c r="E13" s="13">
         <v>87.5</v>
       </c>
-      <c r="G13" s="11">
+      <c r="F13" s="25">
+        <f t="shared" si="4"/>
+        <v>87.833333333333329</v>
+      </c>
+      <c r="H13" s="11">
         <v>90</v>
-      </c>
-      <c r="H13" s="9">
-        <f t="shared" si="1"/>
-        <v>77.5</v>
       </c>
       <c r="I13" s="9">
         <f t="shared" si="0"/>
+        <v>77.5</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="1"/>
         <v>82.5</v>
       </c>
-      <c r="J13" s="9">
-        <f t="shared" si="0"/>
+      <c r="K13" s="9">
+        <f t="shared" si="2"/>
         <v>79.5</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>79.833333333333329</v>
       </c>
     </row>
@@ -5180,23 +5380,27 @@
       <c r="E14" s="13">
         <v>90</v>
       </c>
-      <c r="G14" s="11">
+      <c r="F14" s="25">
+        <f t="shared" si="4"/>
+        <v>90.666666666666671</v>
+      </c>
+      <c r="H14" s="11">
         <v>100</v>
-      </c>
-      <c r="H14" s="9">
-        <f t="shared" si="1"/>
-        <v>80.5</v>
       </c>
       <c r="I14" s="9">
         <f t="shared" si="0"/>
+        <v>80.5</v>
+      </c>
+      <c r="J14" s="9">
+        <f t="shared" si="1"/>
         <v>85.5</v>
       </c>
-      <c r="J14" s="9">
-        <f t="shared" si="0"/>
+      <c r="K14" s="9">
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>82.666666666666671</v>
       </c>
     </row>
@@ -5220,8 +5424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView topLeftCell="G2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5241,13 +5445,14 @@
         <v>0</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -5262,16 +5467,19 @@
       <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5288,23 +5496,27 @@
       <c r="E4" s="10">
         <v>9</v>
       </c>
-      <c r="G4" s="8">
+      <c r="F4" s="25">
+        <f>SUM(D4:E4)/2</f>
+        <v>9</v>
+      </c>
+      <c r="H4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" s="17">
-        <f>C4-9</f>
+      <c r="I4" s="17">
+        <f t="shared" ref="I4:I14" si="0">C4-9</f>
         <v>0</v>
       </c>
-      <c r="I4" s="19">
-        <f t="shared" ref="I4:J14" si="0">D4-9</f>
+      <c r="J4" s="19">
+        <f t="shared" ref="J4:J14" si="1">D4-9</f>
         <v>0</v>
       </c>
-      <c r="J4" s="19">
-        <f t="shared" si="0"/>
+      <c r="K4" s="19">
+        <f t="shared" ref="K4:K14" si="2">E4-9</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f>(I4+J4)/2</f>
+        <f t="shared" ref="L4:L14" si="3">(J4+K4)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -5321,23 +5533,27 @@
       <c r="E5" s="13">
         <v>30</v>
       </c>
-      <c r="G5" s="11">
+      <c r="F5" s="25">
+        <f t="shared" ref="F5:F14" si="4">SUM(D5:E5)/2</f>
+        <v>32.5</v>
+      </c>
+      <c r="H5" s="11">
         <v>10</v>
       </c>
-      <c r="H5" s="17">
-        <f t="shared" ref="H5:H14" si="1">C5-9</f>
+      <c r="I5" s="17">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="I5" s="19">
-        <f t="shared" si="0"/>
+      <c r="J5" s="19">
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="J5" s="19">
-        <f t="shared" si="0"/>
+      <c r="K5" s="19">
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L14" si="2">(I5+J5)/2</f>
+        <f t="shared" si="3"/>
         <v>23.5</v>
       </c>
     </row>
@@ -5354,23 +5570,27 @@
       <c r="E6" s="13">
         <v>40</v>
       </c>
-      <c r="G6" s="11">
+      <c r="F6" s="25">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="H6" s="11">
         <v>20</v>
       </c>
-      <c r="H6" s="17">
+      <c r="I6" s="17">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J6" s="19">
         <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="I6" s="19">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="J6" s="19">
-        <f t="shared" si="0"/>
+      <c r="K6" s="19">
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="L6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
     </row>
@@ -5387,23 +5607,27 @@
       <c r="E7" s="13">
         <v>52</v>
       </c>
-      <c r="G7" s="11">
+      <c r="F7" s="25">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="H7" s="11">
         <v>30</v>
       </c>
-      <c r="H7" s="17">
+      <c r="I7" s="17">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="J7" s="19">
         <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="I7" s="19">
-        <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="J7" s="19">
-        <f t="shared" si="0"/>
+      <c r="K7" s="19">
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
     </row>
@@ -5420,23 +5644,27 @@
       <c r="E8" s="13">
         <v>60.5</v>
       </c>
-      <c r="G8" s="11">
+      <c r="F8" s="25">
+        <f t="shared" si="4"/>
+        <v>64.25</v>
+      </c>
+      <c r="H8" s="11">
         <v>40</v>
       </c>
-      <c r="H8" s="17">
+      <c r="I8" s="17">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="J8" s="19">
         <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="I8" s="19">
-        <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="J8" s="19">
-        <f t="shared" si="0"/>
+      <c r="K8" s="19">
+        <f t="shared" si="2"/>
         <v>51.5</v>
       </c>
       <c r="L8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55.25</v>
       </c>
     </row>
@@ -5453,23 +5681,27 @@
       <c r="E9" s="13">
         <v>66.5</v>
       </c>
-      <c r="G9" s="11">
+      <c r="F9" s="25">
+        <f t="shared" si="4"/>
+        <v>68.5</v>
+      </c>
+      <c r="H9" s="11">
         <v>50</v>
       </c>
-      <c r="H9" s="17">
+      <c r="I9" s="17">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="J9" s="19">
         <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="I9" s="19">
-        <f t="shared" si="0"/>
         <v>61.5</v>
       </c>
-      <c r="J9" s="19">
-        <f t="shared" si="0"/>
+      <c r="K9" s="19">
+        <f t="shared" si="2"/>
         <v>57.5</v>
       </c>
       <c r="L9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>59.5</v>
       </c>
     </row>
@@ -5486,23 +5718,27 @@
       <c r="E10" s="13">
         <v>73</v>
       </c>
-      <c r="G10" s="11">
+      <c r="F10" s="25">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+      <c r="H10" s="11">
         <v>60</v>
       </c>
-      <c r="H10" s="17">
+      <c r="I10" s="17">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="J10" s="19">
         <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="I10" s="19">
-        <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="J10" s="19">
-        <f t="shared" si="0"/>
+      <c r="K10" s="19">
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
     </row>
@@ -5519,23 +5755,27 @@
       <c r="E11" s="13">
         <v>77.5</v>
       </c>
-      <c r="G11" s="11">
+      <c r="F11" s="25">
+        <f t="shared" si="4"/>
+        <v>79.75</v>
+      </c>
+      <c r="H11" s="11">
         <v>70</v>
       </c>
-      <c r="H11" s="17">
+      <c r="I11" s="17">
+        <f t="shared" si="0"/>
+        <v>46.5</v>
+      </c>
+      <c r="J11" s="19">
         <f t="shared" si="1"/>
-        <v>46.5</v>
-      </c>
-      <c r="I11" s="19">
-        <f t="shared" si="0"/>
         <v>73</v>
       </c>
-      <c r="J11" s="19">
-        <f t="shared" si="0"/>
+      <c r="K11" s="19">
+        <f t="shared" si="2"/>
         <v>68.5</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>70.75</v>
       </c>
     </row>
@@ -5552,23 +5792,27 @@
       <c r="E12" s="13">
         <v>82</v>
       </c>
-      <c r="G12" s="11">
+      <c r="F12" s="25">
+        <f t="shared" si="4"/>
+        <v>84.5</v>
+      </c>
+      <c r="H12" s="11">
         <v>80</v>
       </c>
-      <c r="H12" s="17">
+      <c r="I12" s="17">
+        <f t="shared" si="0"/>
+        <v>50.5</v>
+      </c>
+      <c r="J12" s="19">
         <f t="shared" si="1"/>
-        <v>50.5</v>
-      </c>
-      <c r="I12" s="19">
-        <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="J12" s="19">
-        <f t="shared" si="0"/>
+      <c r="K12" s="19">
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75.5</v>
       </c>
     </row>
@@ -5585,23 +5829,27 @@
       <c r="E13" s="13">
         <v>85.5</v>
       </c>
-      <c r="G13" s="11">
+      <c r="F13" s="25">
+        <f t="shared" si="4"/>
+        <v>87.75</v>
+      </c>
+      <c r="H13" s="11">
         <v>90</v>
       </c>
-      <c r="H13" s="17">
+      <c r="I13" s="17">
+        <f t="shared" si="0"/>
+        <v>56.5</v>
+      </c>
+      <c r="J13" s="19">
         <f t="shared" si="1"/>
-        <v>56.5</v>
-      </c>
-      <c r="I13" s="19">
-        <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="J13" s="19">
-        <f t="shared" si="0"/>
+      <c r="K13" s="19">
+        <f t="shared" si="2"/>
         <v>76.5</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>78.75</v>
       </c>
     </row>
@@ -5618,23 +5866,27 @@
       <c r="E14" s="13">
         <v>90.5</v>
       </c>
-      <c r="G14" s="11">
+      <c r="F14" s="25">
+        <f t="shared" si="4"/>
+        <v>93</v>
+      </c>
+      <c r="H14" s="11">
         <v>100</v>
       </c>
-      <c r="H14" s="17">
+      <c r="I14" s="17">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="J14" s="19">
         <f t="shared" si="1"/>
-        <v>59</v>
-      </c>
-      <c r="I14" s="19">
-        <f t="shared" si="0"/>
         <v>86.5</v>
       </c>
-      <c r="J14" s="19">
-        <f t="shared" si="0"/>
+      <c r="K14" s="19">
+        <f t="shared" si="2"/>
         <v>81.5</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
     </row>
@@ -5655,8 +5907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C3:C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5673,14 +5925,14 @@
         <v>6</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="24">
         <v>0.2</v>
       </c>
-      <c r="C3" s="25">
+      <c r="C3" s="26">
         <v>0.97</v>
       </c>
     </row>
@@ -5688,7 +5940,7 @@
       <c r="B4" s="22">
         <v>0.4</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="27">
         <v>1.94</v>
       </c>
     </row>
@@ -5696,7 +5948,7 @@
       <c r="B5" s="22">
         <v>0.6</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="27">
         <v>1.69</v>
       </c>
     </row>
@@ -5704,7 +5956,7 @@
       <c r="B6" s="22">
         <v>0.8</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="27">
         <v>3.26</v>
       </c>
     </row>
@@ -5712,7 +5964,7 @@
       <c r="B7" s="23">
         <v>1</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="27">
         <v>2.5</v>
       </c>
     </row>
@@ -5720,7 +5972,7 @@
       <c r="B8" s="22">
         <v>1.2</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="27">
         <v>2.9</v>
       </c>
     </row>

</xml_diff>